<commit_message>
Updated rps values from NULL to 1 for dominion.
</commit_message>
<xml_diff>
--- a/raw_data/VCEA_goals.xlsx
+++ b/raw_data/VCEA_goals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyung\Documents\GitHub\postgres-etl\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyung\Documents\GitHub\postgres-etl\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDF5F7E-1CA1-4332-8F70-5E23621AC6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7F0128-7C23-4C3C-B226-C2A014022DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2204A34C-DF71-FD48-B1BE-2A1EE1E43562}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -920,7 +920,9 @@
       <c r="B27" s="1">
         <v>0.84</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -935,7 +937,9 @@
       <c r="B28" s="1">
         <v>0.88</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -950,7 +954,9 @@
       <c r="B29" s="1">
         <v>0.92</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -965,7 +971,9 @@
       <c r="B30" s="1">
         <v>0.96</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -980,7 +988,9 @@
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>

</xml_diff>